<commit_message>
excel in convert into mongoDB
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -401,7 +401,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -542,9 +542,60 @@
         <v>Chennai</v>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>ORD50013</v>
+      </c>
+      <c r="B9" t="str">
+        <v>narmadha</v>
+      </c>
+      <c r="C9">
+        <v>2000</v>
+      </c>
+      <c r="D9" t="str">
+        <v>Paid</v>
+      </c>
+      <c r="E9" t="str">
+        <v>sangalpet</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>ORD50013</v>
+      </c>
+      <c r="B10" t="str">
+        <v>ashwini</v>
+      </c>
+      <c r="C10">
+        <v>2500</v>
+      </c>
+      <c r="D10" t="str">
+        <v>Pending</v>
+      </c>
+      <c r="E10" t="str">
+        <v>bangalore</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>ORD50013</v>
+      </c>
+      <c r="B11" t="str">
+        <v>lokesh</v>
+      </c>
+      <c r="C11">
+        <v>2500</v>
+      </c>
+      <c r="D11" t="str">
+        <v>Pending</v>
+      </c>
+      <c r="E11" t="str">
+        <v>bangalore</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E8"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E11"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>